<commit_message>
TestStack.White installed, attempt to launch Notepad failed
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>z nYSKkKU</t>
-  </si>
-  <si>
-    <t>sx qKRbQGVMY</t>
-  </si>
-  <si>
-    <t>SHi3vBN</t>
-  </si>
-  <si>
-    <t>Okl iF k60</t>
-  </si>
-  <si>
-    <t>B9QRV</t>
+    <t xml:space="preserve"> CKO oQf</t>
+  </si>
+  <si>
+    <t>Qt</t>
+  </si>
+  <si>
+    <t>9 fO2v 2x D</t>
+  </si>
+  <si>
+    <t>C P2IWmhi</t>
+  </si>
+  <si>
+    <t>9l</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Homework 24 (Created test data generator which saves files in xlsx format, tests are parametrized by the data obtained from xlsx file)
</commit_message>
<xml_diff>
--- a/data/groups.xlsx
+++ b/data/groups.xlsx
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t xml:space="preserve"> CKO oQf</t>
-  </si>
-  <si>
-    <t>Qt</t>
-  </si>
-  <si>
-    <t>9 fO2v 2x D</t>
-  </si>
-  <si>
-    <t>C P2IWmhi</t>
-  </si>
-  <si>
-    <t>9l</t>
+    <t>LRfY</t>
+  </si>
+  <si>
+    <t>qXC Jc</t>
+  </si>
+  <si>
+    <t>NpLW0dH5Q0EFkF</t>
+  </si>
+  <si>
+    <t>f lmRU</t>
+  </si>
+  <si>
+    <t>RlGpDG4 WYj</t>
   </si>
 </sst>
 </file>
@@ -356,34 +356,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A6"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>